<commit_message>
push 2 desktop (5/6)
</commit_message>
<xml_diff>
--- a/shipClassTests/history.xlsx
+++ b/shipClassTests/history.xlsx
@@ -590,10 +590,10 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -617,10 +617,10 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -644,10 +644,10 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -671,10 +671,10 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -698,10 +698,10 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -770,10 +770,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -797,10 +797,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -824,10 +824,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -851,10 +851,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -878,10 +878,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -986,10 +986,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1103,10 +1103,10 @@
         <v>1</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1130,10 +1130,10 @@
         <v>1</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1157,10 +1157,10 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -1184,10 +1184,10 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1211,10 +1211,10 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1238,10 +1238,10 @@
         <v>1</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1310,19 +1310,19 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -1346,10 +1346,10 @@
         <v>1</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -1373,10 +1373,10 @@
         <v>1</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -1400,10 +1400,10 @@
         <v>1</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -1427,10 +1427,10 @@
         <v>1</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -1454,10 +1454,10 @@
         <v>1</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -1481,10 +1481,10 @@
         <v>1</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -1508,10 +1508,10 @@
         <v>1</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -1526,10 +1526,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1553,10 +1553,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1580,10 +1580,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1607,10 +1607,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1634,10 +1634,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1661,10 +1661,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1688,10 +1688,10 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1715,10 +1715,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1742,10 +1742,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1769,10 +1769,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1823,19 +1823,19 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -1859,10 +1859,10 @@
         <v>1</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -1886,10 +1886,10 @@
         <v>1</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -1913,10 +1913,10 @@
         <v>1</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -1940,10 +1940,10 @@
         <v>1</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57">
         <v>1</v>
@@ -1967,10 +1967,10 @@
         <v>1</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -1994,10 +1994,10 @@
         <v>1</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -2021,10 +2021,10 @@
         <v>1</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60">
         <v>1</v>
@@ -2048,10 +2048,10 @@
         <v>1</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -2093,10 +2093,10 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2120,10 +2120,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -2147,10 +2147,10 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -2174,10 +2174,10 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -2201,10 +2201,10 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2228,10 +2228,10 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -2255,10 +2255,10 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -2282,10 +2282,10 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -2309,10 +2309,10 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -2552,10 +2552,10 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -2714,13 +2714,13 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -2741,13 +2741,13 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -2768,13 +2768,13 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -2795,13 +2795,13 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -2822,13 +2822,13 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -2849,13 +2849,13 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -2930,10 +2930,10 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -2957,10 +2957,10 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -2984,10 +2984,10 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -3011,10 +3011,10 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -3041,19 +3041,19 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98">
         <v>1</v>
       </c>
       <c r="G98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98">
         <f>IF(B98=E98,1,0)</f>
@@ -3068,19 +3068,19 @@
         <v>0</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99">
         <v>1</v>
       </c>
       <c r="G99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99">
         <f>IF(B99=E99,1,0)</f>
@@ -3095,19 +3095,19 @@
         <v>0</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100">
         <v>1</v>
       </c>
       <c r="G100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100">
         <f>IF(B100=E100,1,0)</f>
@@ -3122,19 +3122,19 @@
         <v>0</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101">
         <v>1</v>
       </c>
       <c r="G101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H101">
         <f>IF(B101=E101,1,0)</f>
@@ -3185,7 +3185,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3322,6 +3322,456 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <f>IF(B4 = H4, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <f>IF(B5 = H5, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <f>IF(B6 = H6, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f>IF(B7 = H7, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <f>IF(B8 = H8, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f>IF(B9 = H9, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f>IF(B10 = H10, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <f>IF(B11 = H11, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <f>IF(B12 = H12, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f>IF(B13 = H13, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>